<commit_message>
Improve on scraper pipeline flow
</commit_message>
<xml_diff>
--- a/social_media_scraper/Scraping_Output/instagram_data.xlsx
+++ b/social_media_scraper/Scraping_Output/instagram_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -510,6 +510,300 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>aljazeera</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>a4ffe5f5-c619-412c-8b1d-b7d272f7fd87</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2 hours ago</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>564 likes</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>ينسب اسم المسجد إلى هاشم بن عبد مناف جد الرسول محمد صلى الله عليه وسلم، الذي دفن في الحي بعد وفاته خلال رحلة تجارية في المنطقة.
+#الجزيرة_في_رمضان #معالم_إسلامية</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>aljazeera
+•
+Follow
+Original audio
+564 likes
+aljazeera
+ينسب اسم المسجد إلى هاشم بن عبد مناف جد الرسول محمد صلى الله عليه وسلم، الذي دفن في الحي بعد وفاته خلال رحلة تجارية في المنطقة.
+#الجزيرة_في_رمضان #معالم_إسلامية
+2h
+See translation
+akifmiloud
+صلوات ربي وسلامه عليه 😢
+2h1 likeReply
+See translation
+abo.56ab
+صَلّـوا على المبعوث رحمةً للعالمـين..❤️
+2h2 likesReply
+See translation
+soso1212732
+اللهم صل وسلم على سيدنا محمد ❤️🥺
+2h1 likeReply
+See translation
+er._edres_enze
+😢😢😢😢😢😢😢
+2hReply
+almaz___gainutdinov
+▪️اللهم زدنا عشقاً وحباً في نبيك ﷺ 🤍
+••
+2h1 likeReply
+See translation
+ehab_ihab
+♥️🍉✌🏼🗝️🔻🇵🇸
+1hReply
+hamzah_bin_jazy
+غزه هاشم اسال الله العظيم رب العرش العظيم ان يفرجها عليكم من اوسع ابوابه حسبنا الله ونعم الوكيل
+1hReply
+See translation
+diahrisqiwati
+Yaa Rabb, Allah will help palestine
+2hReply
+maisamimia
+اللهم إن عبادك يبكون شوقا لك ولنصرة دينك فانصرهم بنصرك يارب وانتقم لهم بقدرتك ياعزيز أعز ما أعزك واذل من اذل عبادك المظلومين
+1h1 likeReply
+See translation
+houda_yassminti
+😢😢😢😢😢😢😢 لاحول ولا قوة الا بالله يارب انصرهم
+23mReply
+See translation
+black.g_r
+😭😭😭😭
+2hReply
+n2h.w
+قال النبي (صلى الله عليه وآله): " لا تصلوا علي الصلاة البتراء فقالوا وما الصلاة البتراء؟ قال تقولون " اللهم صل على محمد " وتمسكون بل قولوا اللهم صل على محمد وآل محمد
+2hReply
+zydrkhal
+دمروها اذناب ايران بحماقه 7اكتوبر الله قال اعقل وتوكل مش ورط الشعب واهرب
+24mReply
+See translation
+revolutionuntilvictory
+كيف تعرف خدعة الإنجيليين الصهاينة الذي يحاولون تخريب مشروع ترامب للسلام أو الذين يدعمون كيان الاحتلال مهما فعل .
+ان نجيل متى الإصحاح السابع من ١-٢٩ يكشف هؤلاء . في رقم ١٢: 12 فكل ما تريدون أن يفعل الناس بكم افعلوا هكذا أنتم أيضا بهم، لأن هذا هو الناموس والأنبياء.
+في ٢٤ قيل : 24 فكل من يسمع أقوالي هذه ويعمل بها، أشبهه برجل عاقل، بنى بيته على الصخر.
+لذلك على المتعصبين تعصب اعمى عليهم قرأة إنجيل متى الإصحاح السابع من ١-٢٩ فإن خالفت التعاليم فأنت من رقم ٢٢ -٢٣ في الإصحاح .
+لذلك المسلم يتعايش مع اليهودي و المسيحي بسلام مالم يعتدوا عليه و عندما اضطهد العالم اليهود عاملهم المسلمين بحب و حماهم ثم ظهرت الصهيونية التي بثت الكراهية في كل مكان .
+2h1 likeReply
+See translation
+2 hours ago
+Post</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>2025-03-09 00:51:20</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>video</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>aljazeera</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>6b823bc7-7ebc-4842-929b-8d2aca765f8b</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>15 hours ago</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>4,510 likes</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>قضى جُلّ حياته مغتربًا بسبب معارضته لحكم البعث في #سوريا.. ماذا نعرف عن الداعية والسياسي والمفكر الإسلامي عصام العطار؟⁣
+#الجزيرة_في_رمضان #الجزيرة_بروفايل</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>aljazeera
+•
+Follow
+Original audio
+4,510 likes
+aljazeera
+قضى جُلّ حياته مغتربًا بسبب معارضته لحكم البعث في #سوريا.. ماذا نعرف عن الداعية والسياسي والمفكر الإسلامي عصام العطار؟⁣
+#الجزيرة_في_رمضان #الجزيرة_بروفايل
+15h
+See translation
+sa.abd123
+الاستادذ عصام العطار رحمه الله رحمة واسعة
+5h2 likesReply
+See translation
+sanabel.k
+الابيات الاخيرة مؤثرة جدا 😢
+14h38 likesReply
+See translation
+sa.abd123
+قامة اسلامية كبيرة مفكر يارز ومصلح مميز
+5h7 likesReply
+See translation
+sa.abd123
+بصمات مؤثرة في الاحداث والتاريخ السوري فهو من واجه الالحاد وموامرات التغريب بصوت عال في سوريا
+5h4 likesReply
+See translation
+yana_72m
+رحم الله الداعية المفكر عصام العطار وزوجته بنان الطنطاوي ووالدها الداعية علي الطنطاوي واسكنهم فسيح جنانه
+14h38 likesReply
+See translation
+sa.abd123
+احد ابرز قادة الحركة الاسلامية في سوريا الاموية
+5h4 likesReply
+See translation
+mawadda_abdulhai
+رحمك الله ...آنسك الله...عوضك الله الجنة ...لا والله ما كانت أيامك حلما عشتها يا شيخ بل هي تاريخ مشرف من الإيمان والقوة والثبات على الحق ...
+15h16 likesReply
+See translation
+radwan.dawod
+الغرب لا يريد هؤلاء بالحكم لذلك تراهم بالسجون وفي بلاد المهجر ...
+13h19 likesReply
+See translation
+wisdom.858
+كلها حكومات بالوراثه والسرقه والنهب
+10h1 likeReply
+See translation
+missladybug55
+هذا هو الي كان متزوج بنت المرحوم علي الطهطاوي ، الي اغتالها اعوان الأسد في ألمانيا !!؟ الله يرحمهم برحمته الواسعة ويغفر لهم ويسكنهم فسيح جناته.
+15h21 likesReply
+See translation
+View replies (2)
+reemmarwa72
+سيحان الله فرق الثرى عن الثريا..هوي و اخته نجاح العطار!!!!
+14h3 likesReply
+See translation
+ac110675
+رحمة الله عليه
+15h2 likesReply
+attarloubna
+رحم الله المجاهد والرمز المشرّفة عصام العطار...ليتك شهدت حرية سوريا كما ناضلت كل حياتك في سبيل ذلك..جعلك الله في منازل الشهداء والصديقين
+11h1 likeReply
+See translation
+khair_aljabri
+رحمه الله وأكرم نزله، رجل عظيم
+12h11 likesReply
+See translation
+wareddahabe
+ربي يرحمك يا ابن عمي انت وزوجتك بنان ويسكنكن فسيح جناته
+12h2 likesReply
+See translation
+15 hours ago
+Post</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>2025-03-09 00:51:27</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>video</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Run scraping for Aljazeera posts
</commit_message>
<xml_diff>
--- a/social_media_scraper/Scraping_Output/instagram_data.xlsx
+++ b/social_media_scraper/Scraping_Output/instagram_data.xlsx
@@ -523,7 +523,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>a03cf930-5093-4351-b1b3-1b1b7e5bcec9</t>
+          <t>24ee03b6-58d8-4018-affa-10d16ccf3b67</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -531,7 +531,11 @@
           <t>2025-03-11T22:01:44.000Z</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>163 likes</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr">
         <is>
           <t>NA</t>
@@ -542,11 +546,43 @@
           <t>NA</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>رئيس الهيئة العالمية لأنصار النبي الدكتور محمد الصغير: الأمة المسلمة تعرّضت لامتحان كبير خلال 15 شهرا، لم تنجح فيه إلا الثلة المباركة بغزة وبالعلامة الكاملة.
+#الشريعة_والحياة_في_رمضان #الجزيرة_في_رمضان</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>aljazeera
+•
+Follow
+Original audio
+163 likes
+aljazeera
+رئيس الهيئة العالمية لأنصار النبي الدكتور محمد الصغير: الأمة المسلمة تعرّضت لامتحان كبير خلال 15 شهرا، لم تنجح فيه إلا الثلة المباركة بغزة وبالعلامة الكاملة.
+#الشريعة_والحياة_في_رمضان #الجزيرة_في_رمضان
+20m
+See translation
+h_a_22.23
+الله يحفظ لنا الشيخ عثمان الخميس. مش محتاجين نسمع للاخوان و امثالهم.
+7mReply
+See translation
+iuiu040
+كلام جميل كلام يكتب بماء الذهب
+8mReply
+See translation
+noural6559
+والله سيأتي وعد الله وسنرى رؤوسا مرفوعة مكرّمة ورؤوسا مذلولة محسورة.. اللهم اجعلنا ممن نصرهم يارب
+10m1 likeReply
+See translation
+20 minutes ago
+Post</t>
+        </is>
+      </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>2025-03-12 00:13:10</t>
+          <t>2025-03-12 00:22:11</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -588,15 +624,19 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>85b30c1e-c523-4cd3-a66c-1df3f672ab0f</t>
+          <t>79052833-26d8-4770-a653-1f61328990d9</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2025-03-11T22:01:44.000Z</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
+          <t>2025-03-11T21:30:52.000Z</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>462 likes</t>
+        </is>
+      </c>
       <c r="F3" t="inlineStr">
         <is>
           <t>NA</t>
@@ -607,11 +647,69 @@
           <t>NA</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>قالت وكالة الأنباء اللبنانية إن مسيّرة إسرائيلية شنت غارة على سيارة على طريق رومين وادي دير الزهراني جنوبي البلاد.
+#فيديو</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>aljazeera
+•
+Follow
+Original audio
+462 likes
+aljazeera
+قالت وكالة الأنباء اللبنانية إن مسيّرة إسرائيلية شنت غارة على سيارة على طريق رومين وادي دير الزهراني جنوبي البلاد.
+#فيديو
+51m
+See translation
+saad_monther_alsalem
+😍
+49m1 likeReply
+hazem_hashem1
+حمى الله الحزب من كل شر 💚
+46m3 likesReply
+See translation
+_mohammed_odai_
+وين الحووزب😂😂
+49m2 likesReply
+See translation
+housam_elali
+اذا تابع ل هزب الله….. الله لا يردو و نتمنى المزيد
+48mReply
+See translation
+waliwali1066
+حزب الله يختفي ويتألم 💩💩💩💩💩
+50m5 likesReply
+See translation
+View replies (4)
+ali_alsibai11
+وين الحشد العطواني الشيعي وين ايران؟! لو بس يجون يحشدون للعزاء واللطم على زميرة؟! 😮😂
+50m4 likesReply
+See translation
+llra__95
+هاي الأحداث إن دلت ع شيء حدل ع انو لبنان بدون الحزب مستباح بإختصار الحزب هو حامي الأرض والعرض
+22m1 likeReply
+See translation
+seif.ben
+أين الشيطة البيطة ...ولا شاطرين بتكلموا في الشأن السوري و وين المسيحيين اللي هربوا بأوروبا ويحكوا على سوريا
+41mReply
+See translation
+1mll__llm1
+العدو الاموي واليهودي وجهان لعمله واحده 👍
+44m1 likeReply
+See translation
+josh_grmb17
+16mReply
+51 minutes ago
+Post</t>
+        </is>
+      </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>2025-03-12 00:13:25</t>
+          <t>2025-03-12 00:22:16</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -653,15 +751,19 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>16f7cba3-8c56-4b9f-9cdf-fa9fa1a0790b</t>
+          <t>385e8263-4290-4af9-9268-3d7305d0d54e</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2025-03-11T22:01:44.000Z</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
+          <t>2025-03-11T21:06:21.000Z</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>15,066 likes</t>
+        </is>
+      </c>
       <c r="F4" t="inlineStr">
         <is>
           <t>NA</t>
@@ -672,11 +774,96 @@
           <t>NA</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>الناطق العسكري باسم أنصار الله: قررنا استئناف حظر إبحار السفن الإسرائيلية بالبحرين الأحمر والعربي وباب المندب
+الناطق العسكري باسم أنصار الله: يستمر هذا الحظر حتى فتح معابر قطاع غزة ودخول احتياجاته من غذاء ودواء
+#عاجل</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>aljazeera
+•
+Follow
+Original audio
+15,066 likes
+aljazeera
+الناطق العسكري باسم أنصار الله: قررنا استئناف حظر إبحار السفن الإسرائيلية بالبحرين الأحمر والعربي وباب المندب
+الناطق العسكري باسم أنصار الله: يستمر هذا الحظر حتى فتح معابر قطاع غزة ودخول احتياجاته من غذاء ودواء
+#عاجل
+1h
+See translation
+joulane4356
+رجال صدقو ما عاهدو الله عليه. ونعم الرجال. الله يحفظكم وينصركم
+35m7 likesReply
+See translation
+mh.hazbavi
+👏❤️
+1h3 likesReply
+hamza_taouil1
+الله اكبر الله اكبر
+1h4 likesReply
+See translation
+alghlamajeda
+عاش اليمن ❤️❤️❤️❤️
+1h6 likesReply
+See translation
+ahmad__hamzeh
+رجااال الله إخوان الصدق في يمنا السعيد ❤️
+1h33 likesReply
+See translation
+be_bco
+سدد الله رميكم و أيدكم و أعانكم،و الله اشتقنا لهذي البيانات كثيير 🇾🇪🔥🔥.
+1h52 likesReply
+See translation
+View replies (2)
+qu_rayhana
+اليمن ، السد والسند والناصر والنصير ❤️
+1h117 likesReply
+See translation
+View replies (2)
+bnzhythsbrqm
+إثبتناء ان اليمن إقوئ واشجع دولة عربية بفضل الله ﷻ ثم بفضل السيد القائد حفضة الله ، ❤️
+36m12 likesReply
+See translation
+kursatalperen000
+كما شاركت الشرح الكامل لقصتي
+1h4 likesReply
+See translation
+gtot67
+اذا لم يربيك الزمن فل اليمن يربيك ✌🫡🛐
+32m5 likesReply
+See translation
+dodo_2690
+محلاهم اليمن وأهل اليمن ولا بترددوا لحظة 🥰
+اختي بتحكيلي بالعادة الشعوب بتطلع ضد حكوماتها الا اليمن حكولهم بدنا نضرب نصرة لفلسطين طلعوا مؤيدين ويحكولهم اضربوا 😂😍😍 شعب عجيب الله يجمعنا فيهم واحنا محررين يااارب 💚
+1h38 likesReply
+See translation
+ahmad.hammad3
+قول وفعل 🔥❤️
+1h4 likesReply
+See translation
+mjd.tmeem99
+كفو من رجال اليمن الشجعان ❤️❤️❤️
+1h80 likesReply
+See translation
+View replies (1)
+airport_security1
+عاش اليمن عاش الشعب اليمني عاش كل مقاوم مدافع عند الاقصي وفلسطين 🇾🇪
+1h8 likesReply
+See translation
+quzah1
+قال تعالى " قَالَ سَنَشُدُّ عَضُدَكَ بِأَخِيكَ وَنَجْعَلُ لَكُمَا سُلْطَانًا فَلَا يَصِلُونَ إِلَيْكُمَا ۚ بِآيَاتِنَا أَنتُمَا وَمَنِ اتَّبَعَكُمَا الْغَالِبُونَ " اهل اليمن نعم الاخ و السند
+1h25 likesReply
+See translation
+1 hour ago
+Post</t>
+        </is>
+      </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>2025-03-12 00:13:40</t>
+          <t>2025-03-12 00:22:30</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -718,15 +905,19 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>15b56efe-235d-48cb-82fb-8d53851553dd</t>
+          <t>848d5d60-1029-4ff7-9cd2-293bbd706ee8</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2025-03-11T22:01:44.000Z</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr"/>
+          <t>2025-03-11T20:51:48.000Z</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>1,022 likes</t>
+        </is>
+      </c>
       <c r="F5" t="inlineStr">
         <is>
           <t>NA</t>
@@ -737,11 +928,83 @@
           <t>NA</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>مجلس الوزراء السعودي: نشيد بإجراءات القيادة السورية لصون السلم الأهلي في بلادها واستكمال مسار بناء مؤسسات الدولة من أجل تحقيق الأمن والاستقرار وتلبية تطلعات الشعب السوري، ونجدد دعمنا الكامل لوحدة سوريا وسيادتها وسلامة أراضيها.</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>aljazeera
+•
+Follow
+1,022 likes
+aljazeera
+مجلس الوزراء السعودي: نشيد بإجراءات القيادة السورية لصون السلم الأهلي في بلادها واستكمال مسار بناء مؤسسات الدولة من أجل تحقيق الأمن والاستقرار وتلبية تطلعات الشعب السوري، ونجدد دعمنا الكامل لوحدة سوريا وسيادتها وسلامة أراضيها.
+1h
+See translation
+the.bpakistan
+🇸🇦💚🇵🇰
+1h1 likeReply
+rou2aa_alshahrour
+دعم السعودية للسوريين بالقلب 💚💚الله يجزيكم عنا كل خير 🇸🇦💚
+40m3 likesReply
+See translation
+mr.ahmmedd
+😍😍❤️😍❤️😍❤️
+1h1 likeReply
+yamano.94
+دعم السعودية اثره كبير بالمجتمع الدولي 👌👌
+29m1 likeReply
+See translation
+mo_7amma
+عاشت المملكة العربية السعودية عاشت سوريا 💚💚💚💚💚🇸🇦🇸🇦🇸🇦😍
+1h18 likesReply
+See translation
+20.han0
+❤️
+1h2 likesReply
+ranaal912
+لك كفووو لك الله يديم عز السعودية الف تحية من سوريا الحرة ل احلا مملكة 👏👏🔥🇸🇦💚💚
+59m8 likesReply
+See translation
+the.bpakistan
+موقف حكيم من المملكة يعكس التزامها بدعم الاستقرار والوحدة في المنطقة، وتأصيل دورها الرائد في تعزيز السلام والأمان.
+1h5 likesReply
+See translation
+saud.alyemni
+سوريّـة عشقـنا 🤍💚🖤🇸🇦
+1h1 likeReply
+See translation
+imadox1011
+السعودية بلد جميل يدعم كافة العرب سعودية دولة محبوبة لد شعب المغربي
+1h3 likesReply
+See translation
+jihad_sy92
+💚💚💚💚
+1h2 likesReply
+revolutionuntilvictory
+السعودية ❤️❤️❤️
+1h3 likesReply
+roula_nj
+الله الله عليك يا سعودية 👏👏
+1h3 likesReply
+See translation
+saebaltalib
+بارك الله بكم و جزاكم كل خير و حفظكم و رعاكم ،دمتم بخير و امن و استقرار و سعادة الشعب السعودي
+1h4 likesReply
+See translation
+lhswny890
+دام عزك ياوطن
+31m1 likeReply
+See translation
+1 hour ago
+Post</t>
+        </is>
+      </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>2025-03-12 00:13:55</t>
+          <t>2025-03-12 00:22:34</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -761,7 +1024,7 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>video</t>
+          <t>image</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
@@ -783,15 +1046,19 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0856f681-3c97-4fcd-ab3b-d6b237d5bccd</t>
+          <t>64f2083f-d445-46a3-a05a-a2e19bb8cd41</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2025-03-11T22:01:44.000Z</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr"/>
+          <t>2025-03-11T20:41:21.000Z</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>1,541 likes</t>
+        </is>
+      </c>
       <c r="F6" t="inlineStr">
         <is>
           <t>NA</t>
@@ -802,11 +1069,75 @@
           <t>NA</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>بالمدائح والابتهالات.. فلسطينيون في قطاع غزة يحيون ليالي الشهر الفضيل.
+#الجزيرة_في_رمضان #فيديو</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>aljazeera
+•
+Follow
+Original audio
+1,541 likes
+aljazeera
+بالمدائح والابتهالات.. فلسطينيون في قطاع غزة يحيون ليالي الشهر الفضيل.
+#الجزيرة_في_رمضان #فيديو
+1h
+See translation
+menaelnager
+اللهم صلي عليه وسلم
+1hReply
+See translation
+zaidalbattah321
+❤️❤️
+1hReply
+nadiahilmirahali
+اللهم صل وسلم على محمد وعلى اله وصحبه أجمعين
+1h4 likesReply
+See translation
+hajoura944
+❤️
+6mReply
+houriemasri
+اللهم صل وسلم وبارك على نبينا محمد صلاة تفرج بها عن اهلنا في غزة
+48m1 likeReply
+See translation
+fouad_tazi85
+♥️🇵🇸🇵🇸🇵🇸
+59mReply
+fify.farah
+عليه افضل الصلاة والسلام ربي ينصركم على عدو الامة
+1h1 likeReply
+See translation
+kama_r6379
+ماشاءالله عليهم بالرغم من كل الظروف اللي مرو فيها لكن بمدونا بالطاقه الايجابيه وهمي امس الحاجة الها
+1h2 likesReply
+See translation
+hassanben9998
+غزة العزة ❤️
+1h2 likesReply
+See translation
+asmae_dr_sj
+❤️❤️❤️❤️❤️❤️عليه افضل الصلوات
+31m1 likeReply
+See translation
+fatma.zahra.gaza
+ويصحونا عالسحور ابتهالات والصلاه والسلام على رسول الله
+1h1 likeReply
+See translation
+amir.s.1990_art
+اللهم صل علی محمد و آل محمد ❤️🤲✌️
+1h1 likeReply
+1 hour ago
+Post</t>
+        </is>
+      </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>2025-03-12 00:14:10</t>
+          <t>2025-03-12 00:22:40</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -848,15 +1179,19 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>4b2a0c70-39c9-411f-b306-ff0decee64bf</t>
+          <t>8860866f-15cc-4cf9-bb42-8741b8dbb0b0</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2025-03-11T22:01:44.000Z</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr"/>
+          <t>2025-03-11T20:27:12.000Z</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>1,683 likes</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>NA</t>
@@ -867,11 +1202,70 @@
           <t>NA</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>القيادي في حركة "حـمـ.اس" عبد الرحمن شديد: أرضنا التاريخية في الضفة الغربية والقدس ستظل عصية على الاحتلال.
+#الأخبار</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>aljazeera
+•
+Follow
+Original audio
+1,683 likes
+aljazeera
+القيادي في حركة "حـمـ.اس" عبد الرحمن شديد: أرضنا التاريخية في الضفة الغربية والقدس ستظل عصية على الاحتلال.
+#الأخبار
+1h
+See translation
+basemamasri
+عاشت فلسطين 🇵🇸 حره أبيه محرره بأذن الله❤️
+40m6 likesReply
+See translation
+__ilyasdx26__
+ما أجمل اللغة العربية على ألسنتهم ❤️
+46m5 likesReply
+See translation
+bilal_5_70
+عاشت فلسطين حرة
+1h2 likesReply
+See translation
+twhyrftm
+لا إله الإ انت سبحانك اني كنت من الظالمين اللهم أنصرهم يارب العالمين غزة فلسطين بلد واحد الجزائري 🇵🇸❤️🇩🇿☝️🕌🤲✌️💪💚 الأخضر نحن معك دائما مقاومة
+1h2 likesReply
+See translation
+allab.si2
+بيان مهم للقوات المسلحة اليمنية في تمام الساعة 11:50م، بعد قليل.
+1h1 likeReply
+See translation
+almaz___gainutdinov
+الله اكبر. المقاومة والجهاد في سبيل الله هو الحل الوحيد والاخير .... حل الخلاص من الصهاينة للابد
+1h10 likesReply
+See translation
+View replies (1)
+w32998.gy
+عاااااجل
+العميد يحيى سريع: بيان مهم للقوات المسلحة اليمنية في تمام الساعة 11:50م، بعد قليل.
+1h4 likesReply
+See translation
+View replies (3)
+j_71_1_17_hh
+فلسطينيون باعو ارضهم و باعو نسائهم الي اليهود في غزة 🍆🇵🇸
+1hReply
+See translation
+View replies (1)
+joelzedat
+1hReply
+View replies (1)
+1 hour ago
+Post</t>
+        </is>
+      </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>2025-03-12 00:14:25</t>
+          <t>2025-03-12 00:22:48</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -913,15 +1307,19 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>69ac5e38-5949-4a70-8bd6-84eb82334f4a</t>
+          <t>37f08f43-25bd-48be-9696-bf8c1d8b60e5</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2025-03-11T22:01:44.000Z</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr"/>
+          <t>2025-03-11T20:11:28.000Z</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>677 likes</t>
+        </is>
+      </c>
       <c r="F8" t="inlineStr">
         <is>
           <t>NA</t>
@@ -932,11 +1330,63 @@
           <t>NA</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>كيف نجح السلطان العثماني سليم الأول في دخول دمشق من دون أي مقاومة، وأبقى ولاة الشام على ولاياتهم كما وعدهم؟
+#الجزيرة_في_رمضان #حدث_في_رمضان</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>aljazeera
+•
+Follow
+677 likes
+aljazeera
+كيف نجح السلطان العثماني سليم الأول في دخول دمشق من دون أي مقاومة، وأبقى ولاة الشام على ولاياتهم كما وعدهم؟
+#الجزيرة_في_رمضان #حدث_في_رمضان
+2h
+See translation
+mk9ga
+عاااااجل
+العميد يحيى سريع: بيان مهم للقوات المسلحة اليمنية في تمام الساعة 11:50م، بعد قليل.
+1h1 likeReply
+See translation
+unapologetic.memes
+رحم الله السلطان ''الصاعقة''
+1hReply
+See translation
+orhan_yorukoglu
+Hadimul Haremeyn serefeyin hizmetkârı yüce sultan Yavuz Sultan Selim Han' hazretleri huuu ❤️ cennet mekan olsun
+2h3 likesReply
+wsmlzryy
+لا تنسونا في غزة ؛ اقسم بالله مش لاقيين شيئ نأكله وقت الإفطار والسحور والله تعبنا حسبنا الله ونعم الوكيل في كل من خدلنا 💔💔
+2h6 likesReply
+See translation
+noufs.85
+رحمة الله عليه اول من لقب بـ خادم الحرمين الشريفين وكان حقيق بهذا اللقب .
+2h5 likesReply
+See translation
+View replies (2)
+ali_prince_wwe
+1hReply
+na.sim_official
+😮أردوغان يريد أرض سوريا
+59m1 likeReply
+See translation
+joelzedat
+FROM🇮🇱THE🇮🇱RIVER🇮🇱TO🇮🇱THE🇮🇱SEA🇮🇱
+2hReply
+View replies (2)
+View hidden comments
+These comments were hidden because they may be misleading, offensive or spam. People can still tap to view them.
+2 hours ago
+Post</t>
+        </is>
+      </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>2025-03-12 00:14:40</t>
+          <t>2025-03-12 00:22:54</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -956,7 +1406,7 @@
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>video</t>
+          <t>image</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
@@ -978,15 +1428,19 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>5ee763a2-b7a8-4e0f-bedf-71c00ad50f53</t>
+          <t>4a13d694-7f8d-4e9b-96af-ae6bd97c6334</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2025-03-11T22:01:44.000Z</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr"/>
+          <t>2025-03-11T19:55:42.000Z</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2,994 likes</t>
+        </is>
+      </c>
       <c r="F9" t="inlineStr">
         <is>
           <t>NA</t>
@@ -997,11 +1451,90 @@
           <t>NA</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>عاجل | هيئة البث الإسرائيلية عن مصادر: نتنياهو يستعد خلال الأيام المقبلة للتصديق على خطط العودة للحرب في قطاع غزة.
+#عاجل</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>aljazeera
+•
+Follow
+Original audio
+2,994 likes
+aljazeera
+عاجل | هيئة البث الإسرائيلية عن مصادر: نتنياهو يستعد خلال الأيام المقبلة للتصديق على خطط العودة للحرب في قطاع غزة.
+#عاجل
+2h
+See translation
+f7d___11
+وان عدتم عدنا 🔻
+1h3 likesReply
+See translation
+mk9ga
+عاااااجل
+العميد يحيى سريع: بيان مهم للقوات المسلحة اليمنية في تمام الساعة 11:50م، بعد قليل.
+1h14 likesReply
+See translation
+View replies (1)
+narc.icek
+الله ثم اليمن ثم اليمن ثم اليمن حسبنا الله ونعم الوكيل
+2h1 likeReply
+See translation
+aya_hameed_
+لا تبخلو بالدعاء عليهن بشهر رمضان بلكي يارب يخلصنا منن🥴
+1h10 likesReply
+See translation
+ahmadosama89
+والله غالب على أمره
+2h1 likeReply
+See translation
+abd_rahman_alqaisi_
+مقاومه الفلسطينية في مرصاد 🇵🇸⚔️🫡
+1h11 likesReply
+See translation
+neng_luwi
+Laa haula wala quwwata illa billahil aliyil adzim 🤲
+1h2 likesReply
+See translation
+_free_._palestine
+ربنا يتولى اهلنا في فلسطين
+2h1 likeReply
+See translation
+yaseen_alrafaty
+ذبح فرعون آلاف الذكور خوفاً من أن يأتي موسى ، وعندما جاء موسى .. رباهُ في بيته !
+أقدار اللّٰه نافذة لا محالة فاطمئنوا♥️
+2h226 likesReply
+See translation
+View replies (2)
+_its3a7
+مهلتك تخلص اليوم دير بالك 🔻
+2h6 likesReply
+See translation
+ahmad_hijazi_31
+اي خليه حيلاقي سوريا كلا بسلاحها وتعدادها الكامل 🗡️🗡️
+2h1 likeReply
+See translation
+lmnl1974
+عساك الماحي انت واتباعك
+2h15 likesReply
+See translation
+mamy.toty4
+يا عزيز يا مقتدر خذه أخذا اليما شديدا
+2h70 likesReply
+See translation
+View replies (2)
+haifa_abdallah_saoudi
+2h1 likeReply
+2 hours ago
+Post</t>
+        </is>
+      </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>2025-03-12 00:14:55</t>
+          <t>2025-03-12 00:22:59</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -1043,15 +1576,19 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>12e3966e-2e8e-44e6-ae15-82b921e84f59</t>
+          <t>44ede830-a4b4-4917-83bf-93bee4137b04</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2025-03-11T22:01:44.000Z</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr"/>
+          <t>2025-03-11T19:35:29.000Z</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>5,332 likes</t>
+        </is>
+      </c>
       <c r="F10" t="inlineStr">
         <is>
           <t>NA</t>
@@ -1062,11 +1599,104 @@
           <t>NA</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>لماذا يحظى اتفاق #دمشق و"قوات سوريا الديمقراطية" بتأييد واسع بين السوريين؟
+#الجزيرة_لماذا</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>aljazeera
+•
+Follow
+Original audio
+5,332 likes
+aljazeera
+لماذا يحظى اتفاق #دمشق و"قوات سوريا الديمقراطية" بتأييد واسع بين السوريين؟
+#الجزيرة_لماذا
+2h
+See translation
+hgffy186
+💚💚💛💛💛
+2h1 likeReply
+bayar.miziry
+عاش الامام الثالث عشر احمد الشرع قدس الله سره العظيم ( صلاوات على محمد وال محمد)😍
+2h6 likesReply
+See translation
+View replies (5)
+ri_elamri14
+﷽
+﴿ أَلَم نَشرَح لَكَ صَدرَكَ ۞ وَوَضَعنا عَنكَ وِزرَكَ ۞ الَّذي أَنقَضَ ظَهرَكَ ۞ وَرَفَعنا لَكَ ذِكرَكَ ۞ فَإِنَّ مَعَ العُسرِ يُسرًا ۞ إِنَّ مَعَ العُسرِ يُسرًا ۞ فَإِذا فَرَغتَ فَانصَب ۞ وَإِلى رَبِّكَ فَارغَب ﴾
+❤️ جعلها الله في ميزان حسناتكم 🤲💙
+2h4 likesReply
+See translation
+r.ahmad.1
+وشو من شان الدماء
+2h2 likesReply
+View replies (1)
+nur.zekeriya95
+شاد شكلو تعبان😢😢الله يحمي ويقوي وينصرو💚✌🏻
+2h2 likesReply
+See translation
+faisal8mo
+المهيب ركن احمد الشرع رضي الله عنه كاسر الروافض شرقا وغربا
+2h50 likesReply
+See translation
+View replies (6)
+pg8rs
+الحمدلله 💚
+2h1 likeReply
+dr_karam_kilani
+الله ينصر المسلمين في كل مكان
+2h3 likesReply
+See translation
+ahmad_al.omar
+عندما يتعرض رئيس ما لأزمة يتفاخر بالاعلام باتصال او لقاء بأحد زعماء الدول العظمى ليستمد طاقة وسلطة
+وربما شرعنة اعماله دوليا
+وليأخذ الاوامر ليتصرف
+ولن ينتصر
+القادة الحقيقيون عند الازمات تجدهم في بيوت الله عند السحر يبتهلون الى ربهم ويستخيرونه
+بما تناهت اليه اراؤهم لخير الامة والوطن
+من بيوت الله لا يخرج إلا خيرا وطيبا
+2h2 likesReply
+See translation
+abo_tmara__
+اللهم احفظ سوريا وابعد عنها الفتن والاتهامات الباطلة والي على راسة بطحة يحسس عليها وسمعني احلى (عو عو عو عو) ههههههههههه
+2h11 likesReply
+See translation
+View replies (1)
+ahmad_al.omar
+آآهٍ يا شام!
+يجلس الواحد منّا متابعًا الأحداث لحظةً بلحظة، يفرح قلبه ويقفز من مكانه على كُلّ فتحٍ وانتصارٍ وحدثٍ فارق! ولا يفوته تأمُّل تدبير الله لعباده في ظِلّ تَكالُب الهَمَج من البشر، سبحانه حين قال (مَّا يَفْتَحِ اللَّهُ لِلنَّاسِ مِن رَّحْمَةٍ فَلَا مُمْسِكَ لَهَا) وفي سوريا اليوم؛ رَحَمات نراها ونعلم معناها، وكأنّها هدأة الأنفاس بعد تعب، وهذا لا يعني أنّ الأمر انتهىٰ، مواجهة الباطل قائمة، ولكنّها ضربة ونقطة وهدف، والأيّام بيننا! هنيئًا يا شامنا، ثبّت الله الخُطىٰ، وحمىٰ أهل الثّغور وبارَك.
+2h6 likesReply
+See translation
+View replies (1)
+ftahnamh54.hooajs
+انظروا الى عيونه🙄
+2h1 likeReply
+See translation
+mostafa.mahmoodzade
+کذاب منافق😮😮
+2h4 likesReply
+See translation
+abofayed_85
+احمد الشرع من الاسر في العراق الى رئيس دوله .. إنه من يتقِ ويصبر فإن الله لا يضيع أجر المحسنين .. قصته شبيهه بقصة النبي يوسف عليه السلام
+2h134 likesReply
+See translation
+View replies (19)
+mustafaaa6z
+الرئيس الفاتح المنتصر زعيم الشرق الأوسط والامة العربية احمد الشرع 💚☝️
+2h22 likesReply
+See translation
+View replies (1)
+2 hours ago
+Post</t>
+        </is>
+      </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>2025-03-12 00:15:10</t>
+          <t>2025-03-12 00:23:04</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -1108,15 +1738,19 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>8d779427-62dd-4e12-a732-71fdfd6d98b1</t>
+          <t>e5c950b2-127b-48cc-a4d9-41b02ad15f9e</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2025-03-11T22:01:44.000Z</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr"/>
+          <t>2025-03-11T19:11:51.000Z</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>720 likes</t>
+        </is>
+      </c>
       <c r="F11" t="inlineStr">
         <is>
           <t>NA</t>
@@ -1127,11 +1761,62 @@
           <t>NA</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>مفكر إسلامي من الطراز الأول.. ماذا تعرف عن المفكر الباكستاني فضل الرحمن مالك؟
+#الجزيرة_بروفايل #الجزيرة_في_رمضان</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>aljazeera
+•
+Follow
+Original audio
+720 likes
+aljazeera
+مفكر إسلامي من الطراز الأول.. ماذا تعرف عن المفكر الباكستاني فضل الرحمن مالك؟
+#الجزيرة_بروفايل #الجزيرة_في_رمضان
+3h
+See translation
+hamas_.97
+ماشاءالله
+2h1 likeReply
+ahmed_ansari_99
+رحمه الله تعالى ونفعنا بعلمه
+2h1 likeReply
+See translation
+soso1212732
+ما شاء الله
+3hReply
+See translation
+drmohammedaljaradat
+هذا يؤكد ان اللمو ليس فقط العرب
+3hReply
+See translation
+urgentnews135
+فضل أبو جيف تحليل أمن العراق اعتداءات وج_رائم إيران بأمر أبو محمد الجولاني زعيم المتمردين والي بر دمشق في المنطقة الساحلية بسوريا شاهد ج_رائم داع_ش في السجن والصمت. في وسط الملل استشهد على شواطئ الشام وعلى شواطئ بانياس وفي سفح جبل رخداد سنة 65 بوساطة جماعة أبي محمد الجو_لاني" من حيث حجم الأضرار وعدد الضحايا، فإن هذه الج رائم أكبر بكثير من جريمة ق تل سبايكر.
+1hReply
+See translation
+sayed.ahmad.gh
+القرآن ليس حكراً على تفكر معين بل العالم الإسلامي مزدهر بالمفسرين الذين أتقنوا الفلسفة اليونانية و ألبسوها صبغة إسلامية و استعملوها في التفسير و تبليغ الرسالة.
+2h1 likeReply
+See translation
+alsager599
+بعد هذا كله هل دفن مع المسلمين ولا مع الكفار كل شي بالخاتمه (المقبره التي دفن فيها بامريكا هل تخص المسلمين ولا الكفار )
+2hReply
+See translation
+abdollahaboahmad
+الحمد لله أن إسلامنا ليس فلسفة ولا هرطقة ولا سفسطة، بل هو أحكام يفهما العالم والعامي بسهولة ويسر ودون تقعر ولا تقعيد، وهو حياة المسلم بل والبشرية لو التزموا أحكامه في كل زمان ومكان، لهذا يتهم من رفض سفسطته بالتشدد..
+3hReply
+See translation
+3 hours ago
+Post</t>
+        </is>
+      </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>2025-03-12 00:15:25</t>
+          <t>2025-03-12 00:23:09</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -1173,15 +1858,19 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>37d8b389-02aa-4620-bbeb-568da9c252d1</t>
+          <t>d3d26d6b-a648-455b-851c-537ddabb6df2</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2025-03-11T22:01:44.000Z</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr"/>
+          <t>2025-03-11T18:51:37.000Z</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>467 likes</t>
+        </is>
+      </c>
       <c r="F12" t="inlineStr">
         <is>
           <t>NA</t>
@@ -1192,11 +1881,61 @@
           <t>NA</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>الحكومة السورية تجتمع مع وجهاء السويداء لدمج مؤسسات المحافظة ضمن الدولة، واستشـ.ـهاد 11 فلسطينيا بقصف إسرائيلي على #غزة خلال يوم واحد.⁣
+⁣
+الخبر في قصة بـ #إيجاز</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>aljazeera
+•
+Follow
+Original audio
+467 likes
+aljazeera
+الحكومة السورية تجتمع مع وجهاء السويداء لدمج مؤسسات المحافظة ضمن الدولة، واستشـ.ـهاد 11 فلسطينيا بقصف إسرائيلي على #غزة خلال يوم واحد.⁣
+⁣
+الخبر في قصة بـ #إيجاز
+3h
+See translation
+jodyssg
+بني معروف طول عمرهم مع الثورة السوريه💚
+3h1 likeReply
+See translation
+urgentnews135
+فضل أبو جيف تحليل أمن العراق اعتداءات وج_رائم إيران بأمر أبو محمد الجولاني زعيم المتمردين والي بر دمشق في المنطقة الساحلية بسوريا شاهد ج_رائم داع_ش في السجن والصمت. في وسط الملل
+استشهد على شواطئ الشام وعلى شواطئ بانياس وفي سفح جبل رخداد سنة 65 بوساطة جماعة أبي محمد الجو_لاني"
+من حيث حجم الأضرار وعدد الضحايا، فإن هذه الج رائم أكبر بكثير من جريمة ق تل سبايكر.
+1hReply
+See translation
+weam7221
+اشو عم تشربوا حشيش قناة الجزيرة 😂😂😂😂
+3hReply
+See translation
+fifiluthfiati9
+Free Palestine 🤲☝️✊💪🇵🇸
+Save Suriah 🤲☝️✊💪
+3h1 likeReply
+ahmet._.karcum
+هناك دوله تراقب وتلطم بصمت 🤐
+3hReply
+See translation
+bdlrzq.lqwsmy
+اسال الله في هالايام الفضيله والساعه المباركه ان يسلط عليكم الامراض والزلازل والكورونا وربنا يهلكهم في الدنيا قبل الاخره اللهم ارينا يا رب فيهم عجائب قدرتك انهم لا يعجزونك اللهم استجب اللهم استجب اللهم استجب اللهم امين يا رب العالمين
+1hReply
+See translation
+joelzedat
+3hReply
+3 hours ago
+Post</t>
+        </is>
+      </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>2025-03-12 00:15:39</t>
+          <t>2025-03-12 00:23:14</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1238,15 +1977,19 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>9bd7551a-1d2e-4d7e-a565-748e72a02e09</t>
+          <t>63dffd2e-29cb-4d3c-b0df-515aa0b9f786</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2025-03-11T22:01:44.000Z</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr"/>
+          <t>2025-03-11T18:30:36.000Z</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2,397 likes</t>
+        </is>
+      </c>
       <c r="F13" t="inlineStr">
         <is>
           <t>NA</t>
@@ -1257,11 +2000,107 @@
           <t>NA</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>عاجل | بيان أمريكي أوكراني مشترك بعد اجتماع السعودية: اتخذنا خطوات مهمة باتجاه تحقيق سلام دائم في أوكرانيا.
+📌 الخارجية الأمريكية: أوكرانيا أعربت عن استعدادها للموافقة على مقترح أمريكي بوقف فوري لإطلاق النار مدته 30 يوما.
+📌 بيان أمريكي أوكراني مشترك: الولايات المتحدة ستوقف فورا تعليق المساعدات والتبادل الاستخباري مع أوكرانيا.
+📌 زيلنسكي: إذا وافقت روسيا على الهدنة ففي تلك اللحظة سيسود الهدوء فعليا.
+📌 زيلنسكي: استئناف المساعدات الأمريكية لأوكرانيا كان عاملا مهما في التوصل لاتفاق.
+📌 زيلنسكي: أوكرانيا مستعدة للسلام وعلى روسيا إعلان موقفها من إنهاء الحرب أو مواصلتها.
+📌 زيلنسكي: اقترحنا على واشنطن هدنة جوية وبحرية وإجراءات حقيقية لبناء الثقة بما فيها إطلاق سراح أسرى.
+#عاجل</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>aljazeera
+•
+Follow
+Original audio
+2,397 likes
+aljazeera
+عاجل | بيان أمريكي أوكراني مشترك بعد اجتماع السعودية: اتخذنا خطوات مهمة باتجاه تحقيق سلام دائم في أوكرانيا.
+📌 الخارجية الأمريكية: أوكرانيا أعربت عن استعدادها للموافقة على مقترح أمريكي بوقف فوري لإطلاق النار مدته 30 يوما.
+📌 بيان أمريكي أوكراني مشترك: الولايات المتحدة ستوقف فورا تعليق المساعدات والتبادل الاستخباري مع أوكرانيا.
+📌 زيلنسكي: إذا وافقت روسيا على الهدنة ففي تلك اللحظة سيسود الهدوء فعليا.
+📌 زيلنسكي: استئناف المساعدات الأمريكية لأوكرانيا كان عاملا مهما في التوصل لاتفاق.
+📌 زيلنسكي: أوكرانيا مستعدة للسلام وعلى روسيا إعلان موقفها من إنهاء الحرب أو مواصلتها.
+📌 زيلنسكي: اقترحنا على واشنطن هدنة جوية وبحرية وإجراءات حقيقية لبناء الثقة بما فيها إطلاق سراح أسرى.
+#عاجل
+Edited · 3h
+See translation
+lshfy3660
+ماشاءالله تبارك وغزه الحصار لاحول ولا قوة الا بالله العلي العظيم حسبي الله ونعم الوكيل
+1h1 likeReply
+See translation
+ben_omar_abkal
+وما محل قريش في الاعراب
+3h2 likesReply
+See translation
+fati.manour64
+وعليكم بتحقيق السلام لذوي القربى
+3h1 likeReply
+See translation
+mr_bwsmrh
+اه يا غزه اه لك الله😢
+3h1 likeReply
+See translation
+setif0462
+وفلسطين غير معنية من وقف الحرب والإبادة
+2h1 likeReply
+See translation
+modi__993
+غزه يا بن سلمان
+3h1 likeReply
+gramlink.academy
+اه يا غزة لكي الله ، والنعم برب العباد
+3h26 likesReply
+See translation
+View replies (1)
+akkouche__97
+غزة لا تعنيكم !
+3h22 likesReply
+See translation
+View replies (1)
+ettahiri477
+😢وغزة 💔💔
+1h1 likeReply
+See translation
+a_a20hm
+بالسعودية يتم حلب اوكرانيا
+2h1 likeReply
+See translation
+joujou_the_king
+إنتظروا فقط بعد أن يرد بوتين على الهجوم الأخير الأوكراني بعدها اجتمعوا وقرروا يا صهابنة ✅
+3h3 likesReply
+See translation
+View replies (1)
+khaledinho_qa
+وغزة يا موسم الرياض ؟! أليست أولى؟؟
+3h9 likesReply
+See translation
+View replies (2)
+zakmous
+حسبي الله ونعم الوكيل اين انتم من غزه
+3h1 likeReply
+See translation
+berghoutim
+المجد لروسيات
+3h2 likesReply
+See translation
+View replies (1)
+hudalabwam
+والسعوديه اين موقفها من غزة وفلسطين حسبنا الله ونعم الوكيل
+2h1 likeReply
+See translation
+3 hours ago
+Post</t>
+        </is>
+      </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>2025-03-12 00:15:54</t>
+          <t>2025-03-12 00:23:19</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
@@ -1303,15 +2142,19 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>f8b4f892-e7c0-49fa-b0d8-0c1c405de4b1</t>
+          <t>e195bbd8-87b5-428d-967c-f5b8d58bc150</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2025-03-11T22:01:44.000Z</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr"/>
+          <t>2025-03-11T18:13:28.000Z</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>4,175 likes</t>
+        </is>
+      </c>
       <c r="F14" t="inlineStr">
         <is>
           <t>NA</t>
@@ -1322,11 +2165,82 @@
           <t>NA</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>نظم متضامنون مع فلسطين مظاهرة في مدينة نيويورك الأمريكية يوم الاثنين، احتجاجا على احتجاز السلطات الناشط الفلسطيني محمود خليل وإلغاء بطاقته للإقامة الدائمة بالولايات المتحدة.
+#فيديو</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>aljazeera
+•
+Follow
+Original audio
+4,175 likes
+aljazeera
+نظم متضامنون مع فلسطين مظاهرة في مدينة نيويورك الأمريكية يوم الاثنين، احتجاجا على احتجاز السلطات الناشط الفلسطيني محمود خليل وإلغاء بطاقته للإقامة الدائمة بالولايات المتحدة.
+#فيديو
+4h
+See translation
+fadimetorun.83
+🙌❤️🇵🇸🇵🇸🇵🇸
+3h2 likesReply
+eman7sn55
+هل ستصدرون قرار تهجير الشعب الأمريكي لدعمه لفلسطين ومساندة القاتل الأسلحة المدمرة
+3h5 likesReply
+See translation
+maryoom13101
+وعي الأجانب في قلبي ❤️‍🩹❤️‍🩹❤️‍🩹🥹🥹
+4h7 likesReply
+See translation
+quran.islam10
+قال رسول الله ﷺ:"لقد رأيتُ رجلًا يتقلَّبُ في الجنَّةِ ، في شجرةٍ قطعَها من ظهرِ الطريقِ ، كانت تُؤذي النَّاس"
+لا تستصغر فعل الخير لا تدري بأي عمل تدخل الجنة♥️
+4h13 likesReply
+See translation
+ilhamouall
+أرادوا مسح فلسطين ، فأصبح العالم كله فلسطين
+4h45 likesReply
+See translation
+berghoutim
+لا لسياسة الكيل بمكيالين،فلسطين عربية وستبقى عربية من النهر الى البحر
+3h4 likesReply
+See translation
+cp_35k
+هؤلاء اشرف من ال سعود تاركين غزة ويبحثون عن سلام دائم في اوكرانيا
+2h9 likesReply
+See translation
+jihad__waleed
+ما لا يستطيع حكام العرب ان يفعله
+3h8 likesReply
+See translation
+revolutionuntilvictory
+في ظاهرة تاريخيّة اكثر من ٧٠٪؜ من الأمريكيين مؤيدون لفلسطين. كلما زادت القسوة على مناصرين فلسطينيين فإن الصامتون يخرجون عن صمتهم وينضمون للحق الفلسطيني ضد الباطل الإسرائيلي الذي ينفق الإعلام الصهيوني عليه مليارات الدولارات. كلها ذهبت هباء منثورة مقابل دماء الضحايا الفلسطينيين التي سفكت على يد ا-شر المخلوقات . ان الإعلام الصهيوني يزور كل شيء و يستهدف عقول الأمريكيين لكي يخربها .
+4h1 likeReply
+See translation
+hiduplive
+God bless you all the beautiful souls ❤️ thank you for standing with humanity ❤️❤️❤️
+2h1 likeReply
+keith__johnston
+Lunatics
+3hReply
+View replies (1)
+lyl0p
+والمسلمين مشغولين انت سني انت شيعي والكافر يدافع عن غزة
+3h2 likesReply
+See translation
+View replies (1)
+joelzedat
+4hReply
+View replies (1)
+4 hours ago
+Post</t>
+        </is>
+      </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>2025-03-12 00:16:09</t>
+          <t>2025-03-12 00:23:24</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1368,15 +2282,19 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>505ca249-1d37-4bde-8bd8-6d357045f705</t>
+          <t>3c0db4c4-2b6b-42ea-acab-4c22ebb913ca</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2025-03-11T22:01:44.000Z</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr"/>
+          <t>2025-03-11T17:48:32.000Z</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>579 likes</t>
+        </is>
+      </c>
       <c r="F15" t="inlineStr">
         <is>
           <t>NA</t>
@@ -1387,11 +2305,45 @@
           <t>NA</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>جراء ارتفاع درجات الحرارة وذوبان التربة الصقيعية.. ما الدول التي "ستستفيد" من التغير المناخي؟
+#رقمي</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>aljazeera
+•
+Follow
+Original audio
+579 likes
+aljazeera
+جراء ارتفاع درجات الحرارة وذوبان التربة الصقيعية.. ما الدول التي "ستستفيد" من التغير المناخي؟
+#رقمي
+4h
+See translation
+athkarr.quran
+💛
+شجرة ظلّها دائم، وساقُها من ذهب:
+سبحان الله، الحمدلله، لا إله إلا الله، والله أكبر
+4h2 likesReply
+See translation
+abdellah2_sadik
+نسيت احتمال اختفاء العالم العربي بفعل التغير المناخي و التصحر،و هو احتمال كبير
+3hReply
+See translation
+gelan490
+⛔تأخير.. ⛔تكبير.. ⛔
+4hReply
+See translation
+4 hours ago
+Post</t>
+        </is>
+      </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>2025-03-12 00:16:24</t>
+          <t>2025-03-12 00:23:28</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1433,15 +2385,19 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>75a6e292-c5f5-415c-825c-03c702c07f1a</t>
+          <t>0c13a55e-acf4-4ffe-9e7f-4c9d23ae8943</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2025-03-11T22:01:44.000Z</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr"/>
+          <t>2025-03-11T17:26:46.000Z</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>6,815 likes</t>
+        </is>
+      </c>
       <c r="F16" t="inlineStr">
         <is>
           <t>NA</t>
@@ -1452,11 +2408,86 @@
           <t>NA</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>عاجل | حـمـ.اس: ندعو إلى مواصلة الرباط في المسجد الأقصى والتصدي لمحاولات الاحتلال والمستوطنين تدنيسه، ونحذر من سعي الاحتلال لتشريع ما يسمى بمخطط القدس الكبرى.
+#عاجل</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>aljazeera
+•
+Follow
+Original audio
+6,815 likes
+aljazeera
+عاجل | حـمـ.اس: ندعو إلى مواصلة الرباط في المسجد الأقصى والتصدي لمحاولات الاحتلال والمستوطنين تدنيسه، ونحذر من سعي الاحتلال لتشريع ما يسمى بمخطط القدس الكبرى.
+#عاجل
+Edited · 4h
+See translation
+nabil_aorich
+ونحن منصتون لحـ .ماس
+4h1 likeReply
+See translation
+ayman7100
+عباس راضع من النتن كيف بدكم يوقف التنسيق وهو ابنه بالرضاعه
+4h1 likeReply
+See translation
+lolagazaly
+الله معكم وناصركم 💚💚🌴🇯🇴🤲
+4h3 likesReply
+See translation
+ilhamouall
+قال مولانا عَز وجل: ذَٰلِكُمۡ وَأَنَّ ٱللَّهَ مُوهِنُ كَيۡدِ ٱلۡكَٰفِرِينَ (18) إِن تَسۡتَفۡتِحُواْ فَقَدۡ جَآءَكُمُ ٱلۡفَتۡحُۖ وَإِن تَنتَهُواْ فَهُوَ خَيۡرٞ لَّكُمۡۖ وَإِن تَعُودُواْ نَعُدۡ وَلَن تُغۡنِيَ عَنكُمۡ فِئَتُكُمۡ شَيۡـٔٗا وَلَوۡ كَثُرَتۡ وَأَنَّ ٱللَّهَ مَعَ ٱلۡمُؤۡمِنِينَ
+4h12 likesReply
+ilhamouall
+قال الله تعالى وَدَّ الَّذِينَ كَفَرُوا لَوْ تَغْفُلُونَ عَنْ أَسْلِحَتِكُمْ وَأَمْتِعَتِكُمْ فَيَمِيلُونَ عَلَيْكُم مَّيْلَةً وَاحِدَةً صدق الله العظيم
+4h30 likesReply
+See translation
+View replies (3)
+mostafamostafa9266
+يجيب اصطياد نتين هادا
+4h1 likeReply
+See translation
+benz.abdeladim
+التقاعس و التخاذل العربي هو سبب ذالك زيادة على تواطئ صهاينة العرب في هذه الجريمة
+4h1 likeReply
+See translation
+abooda761
+حسبي الله
+4h1 likeReply
+See translation
+ma_nar_20a
+الى متى هذا سكوت من حكام العرب ومسجدنا الاقصى يدنس من اليهود
+4h30 likesReply
+See translation
+View replies (11)
+rahim_dz_7
+🔴 حركة حماس: إمعان الاحتلال في حربه ضد مقدساتنا ومساجدنا إرهاب صهيوني وانتهاك لكل الأعراف والشرائع السماوية
+▫️نحذر من سعي الاحتلال لتشريع ما يسمى بمخطط القدس الكبرى واستمرار إغلاق معابر قطاع غزة جريمة حرب وعقاب جماعي
+▫️ندعو الوسطاء إلى ممارسة كل الضغوط على نتنياهو وحكومته للالتزام بشروط وقف إطلاق النار
+▫️نأمل أن تسفر مساعي المبعوث الأمريكي عن بدء مفاوضات المرحلة الثانية من اتفاق وقف إطلاق النار
+▫️نُطالب المجتمع الدولي بالتحرك الجاد للضغط على الاحتلال لوقف جرائمه وانتهاكاته الخطيرة
+4h1 likeReply
+See translation
+mostafa.mahmoodzade
+وین حکام وسلاطین و......عرب😮😮
+4h2 likesReply
+See translation
+lrhmn18_8
+عندما يذكر الحق، تذكر فل سطين وعندما يُذكر الصمود، تذكر غزة🔥🔥
+4h3 likesReply
+See translation
+omessa130
+4h3 likesReply
+4 hours ago
+Post</t>
+        </is>
+      </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>2025-03-12 00:16:39</t>
+          <t>2025-03-12 00:23:33</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1498,15 +2529,19 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>761e54ce-8847-49b9-aefc-ee67a58b0748</t>
+          <t>ca7603d2-11e6-4545-9710-a593c26532b3</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2025-03-11T22:01:44.000Z</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr"/>
+          <t>2025-03-11T17:06:02.000Z</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>1,978 likes</t>
+        </is>
+      </c>
       <c r="F17" t="inlineStr">
         <is>
           <t>NA</t>
@@ -1517,11 +2552,78 @@
           <t>NA</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>عاجل | الجيش الإسرائيلي: إصابة إسرائيلية بجروح بعد رشق مركبتها بالحجارة قرب مستوطنة أفيتار شمال الضفة الغربية.
+#عاجل</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>aljazeera
+•
+Follow
+Original audio
+1,978 likes
+aljazeera
+عاجل | الجيش الإسرائيلي: إصابة إسرائيلية بجروح بعد رشق مركبتها بالحجارة قرب مستوطنة أفيتار شمال الضفة الغربية.
+#عاجل
+5h
+See translation
+maryoom13101
+يا رب تكون الحجارة بخير
+4h18 likesReply
+See translation
+al.kilani0
+الحمدلله
+5h2 likesReply
+rikoarianto2025
+الله أكبر ☝️☝️☝️🔻🔻🔻🔥🔥🔥
+3h2 likesReply
+shwayyat1
+فشخها؟
+5h2 likesReply
+See translation
+mohamedemad8193
+لا أمان لكم في العالم فهذا حصاد ماقترفتموه
+5h15 likesReply
+See translation
+abdelhakhakan
+ان شاء الله الاصابات تكون خطيرة اكثر مما نتوقع
+4h3 likesReply
+See translation
+shahed_hosein
+عاش 🔥
+5h2 likesReply
+See translation
+gass_em679
+- نحذر من خطورة وتداعيات العدوان الإسـ.رائيلي لتهجير شعبنا
+- مخططات التهجير تستهدف أمن الدول العربية
+- أرضنا التاريخية في الضفة الغربية والقـ.دس ستظل عصية على الاحتـ.ـلال
+- إمعان الاحـ.ـتلال في حربه ضد مقدساتنا ومساجدنا إرهـ.اب صهـ.ـيوني وانتهاك لكل الأعراف والشرائع السماوية
+- نطالب المجتمع الدولي بالتحرك الجاد للضغط على الاحتـ.ـلال لوقف جرائمه وانتهاكاته الخطيرة
+- نتعامل بكل مسؤولية وإيجابية مع مفاوضات وقف إطلاق النار
+- ندعو للضغط على الاحتـ.ـلال للسماح بعمل وسائل الإعلام لتغطية الحقيقة
+- ندعو القوى الحية في الضفة والقدس إلى توحيد الكلمة وتعزيز الصمود والمقاومة
+- ندعو السلطة الفلسطينية إلى التوقف الفوري عن سياسة التنسيق الأمني وملاحقة المقاومين
+- ندعو إلى مواصلة #الرباط في المسجد الأقصى والتصدي لمحاولات الاحتلال والمستوطنين تدنيسه
+4h1 likeReply
+See translation
+iraq_a09
+والله ابطال بالحجارة😂
+5hReply
+See translation
+mustafaaa6z
+اللهم زيد من جرحاهم وقتلاهم ولا ترحم فيهم احده 🔥
+5h4 likesReply
+See translation
+5 hours ago
+Post</t>
+        </is>
+      </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>2025-03-12 00:16:54</t>
+          <t>2025-03-12 00:23:38</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1563,15 +2665,19 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>033e29ce-6381-42f8-a23b-1dbabdbc851c</t>
+          <t>e376219b-b911-4567-adb2-064dfa9862bb</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2025-03-11T22:01:44.000Z</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr"/>
+          <t>2025-03-11T16:40:25.000Z</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>1,891 likes</t>
+        </is>
+      </c>
       <c r="F18" t="inlineStr">
         <is>
           <t>NA</t>
@@ -1582,11 +2688,73 @@
           <t>NA</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>عاجل | مراسل #الجزيرة: الصليب الأحمر الدولي يتسلم 4 أسرى لبنانيين من إسرائيل.⁣
+⁣
+#عاجل</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>aljazeera
+•
+Follow
+Original audio
+1,891 likes
+aljazeera
+عاجل | مراسل #الجزيرة: الصليب الأحمر الدولي يتسلم 4 أسرى لبنانيين من إسرائيل.⁣
+⁣
+#عاجل
+5h
+See translation
+hawraa_alsalman92
+قصدكم الصليب الاسرائيلي
+5hReply
+See translation
+am7f7
+الجزيرة شو مغلسه عن الأحداث بسوريا شنو العلويين مو بشر
+5h14 likesReply
+See translation
+View replies (20)
+nharyazan
+يا جزيرة شوفو أخبار سورية انا سوري ساكن بريف دمشق سمعان صوت طيران على الأكيد اسرائيلي
+5h6 likesReply
+See translation
+View replies (1)
+hosse.in7178
+ماذا كانت نتيجة هجوم 7 أكتوبر بالنسبة للفلسطينيين؟
+5h2 likesReply
+See translation
+View replies (6)
+tameemabojazar
+غارات عنيفة على اليمن..
+تغطية الاحداث بالستوري 🚨
+5h2 likesReply
+See translation
+revolutionuntilvictory
+سوف يدرك العالم قريبا ان تفكيك اسرائيل و ارسال مكونتها كل إلى بلده الأصلية هو افضل شيء للإنسانية. شعوب العالم يوم بعد يوم تترسخ لديهم ان إسرائيل كيان شرير متكامل خدع العالم و أنه يشوه سمعة اليهود ويشكل خطر عليهم لذلك ربط إسرائيل باليهود يجب ان يصنف معاداة للسامية . للبنان حق اسر صهاينة ايضا . هل اسرائيل التي تنسب نفسها لليهودية . عندما تقتل الإسرائيليين في نظام هنيبعل تكون قد خالفت شريعة اليهود وقتلتهم عمدا ؟ و ما حكم القتل العمد في شريعة اليهود ؟
+5h1 likeReply
+See translation
+sama_____29
+The tunnels of Ahmed al-Sharaa and his government. With the Kurds. The same tunnels of Saddam Hussein with the Kurds in 1970. A few years later, Saddam Hussein bombed the Kurds in Iraq with chemical weapons and a million Kurds were martyred, including children, women, youth, elderly people, and pregnant women.
+5hReply
+View replies (1)
+sama_____29
+The new Syrian government is the government of Hay'at Tahrir al-Sham. It gave security to the Alawites and Christians, and then. It asked them to surrender their weapons, and then we saw how. The state of Ahmed al-Sharaa. It committed genocide and mass graves against the Syrian people, Alawites and Christians. And the same will happen to the Druze and Kurds. The same thing that happened to the Alawites. Because the Umayyad government has no security and no covenants.
+5hReply
+View replies (2)
+sama_____29
+أنفاق احمد الشرع وحكومته. مع الاكراد. نفس انفاق صدام حسين مع الاكراد 1970. بعدها بكم سنة صدام حسين قصف الاكراد في العراق بالسلاح الكيميائي واستشهد مليون كردي من أطفال ونساء وشباب وكبار السن ونساء حوامل
+5h1 likeReply
+See translation
+5 hours ago
+Post</t>
+        </is>
+      </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>2025-03-12 00:17:09</t>
+          <t>2025-03-12 00:23:43</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
@@ -1628,15 +2796,19 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>e50502fd-5736-4725-a0e1-849fc859fdf4</t>
+          <t>1d70aa9e-d07d-4672-bc75-7af23d1551e3</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2025-03-11T22:01:44.000Z</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr"/>
+          <t>2025-03-11T16:16:26.000Z</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>3,269 likes</t>
+        </is>
+      </c>
       <c r="F19" t="inlineStr">
         <is>
           <t>NA</t>
@@ -1647,11 +2819,122 @@
           <t>NA</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>فرحة معلم يمني يبيع الليمون في الشارع، بعد حصوله على هدية من أحد طلابه السابقين بطريقة غير مباشرة.⁣
+⁣
+القصة في #شبكات مع #أحمد_فاخوري على شاشة #الجزيرة⁣
+⁣
+#شبكات_الجزيرة</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>aljazeera
+and
+ahmad_fakhouri_official
+Original audio
+3,269 likes
+aljazeera
+فرحة معلم يمني يبيع الليمون في الشارع، بعد حصوله على هدية من أحد طلابه السابقين بطريقة غير مباشرة.⁣
+⁣
+القصة في #شبكات مع #أحمد_فاخوري على شاشة #الجزيرة⁣
+⁣
+#شبكات_الجزيرة
+6h
+See translation
+en_rihan
+لا حول ولا قوة إلا بالله العلي العظيم وحسبي الله و نعم الوكيل على كل من حاربهم وكل من جوعهم حسبي الله و نعم الوكيل
+6h1 likeReply
+See translation
+s11af_albahri
+لك الله ي بلادي 😢❤️
+4h10 likesReply
+See translation
+sera_alariqi
+الله لا سامح من كان السبب معلمينا صاروا مذلولين 💔💔💔💔ربي ييسر لهم
+4h4 likesReply
+See translation
+roaa_abd.o
+خلصت من سوريا بلشت باليمن يلا لنشوف اخرها
+5h9 likesReply
+See translation
+View replies (2)
+shwayyat1
+قف للمعلم وفيه التبجيلا كاد المعلم أن يكون رسولا
+6h3 likesReply
+See translation
+sozana87
+يا اهل اليمن مو ناسيينكن انتو بالقلب والله ، ربي يفرجا عليكن و ينتقم من اعدائكن و يقويكن عليهن 🤲💚🥹
+5h15 likesReply
+See translation
+View replies (1)
+bkry.10
+إذا كان راتب العسكري يفوق راتب المعلم أضعافا مضاعفة كيف سيُبنى جيل يحب حمل القلم بدلاً من حمل السلاح؟ لكم من الله ماتستحقون يا من أوصلتم معلمينا وبلدنا إلى هذا المستوى.
+5h47 likesReply
+See translation
+View replies (9)
+_.llah_
+لعائن الله على الدول الصهيونية التي تعاونت للحر،ب على اليمن.
+5h4 likesReply
+See translation
+njnr.i
+يااااااااااااااااارب نحن من اليمن
+5h9 likesReply
+See translation
+View replies (4)
+lo1mo27
+ببنما في مناطق الشمال المعلم لايستلم أي راتب😢
+5h4 likesReply
+See translation
+View replies (2)
+hhhhsgga
+( الى اصحاب القول الرحيمة انقذوا مجد )
+💉 2.1 مليون دولار .. رقم ثقيل، لكنه قد يكون الفرق بين الحياة والموت 💔
+⚠️ ارجو واتمنى من الجميع مشاركة هذا المنشور .. فقد تكون يدك هي من تكتب النجاة للطفل مجد ⚠️
+2 مليون دولار ليس مجرد رقم يُكتب على ورق، وليس مبلغًا يمكن جمعه بسهولة .. إنه السد الفاصل بين طفل بريء والحياة.
+إنه العائق الذي يقف بين مجد وبين أن يتنفس بحرية، بينه وبين أن يحرك يديه الصغيرتين، بينه وبين أن ينطق "أمي، أبي" لأول مرة.
+🔴 مجد ثروت عبدالله عنبول، عمره عام وشهران فقط .. لم يختر أن يولد بهذا المرض القاتل، ضمور العضلات الشوكي - النوع الأول، الذي سلبه القدرة على الحركة والتنفس، وحرمه من الضحك واللعب، وسرق منه طفولته قبل أن تبدأ.
+اليوم، يرقد في مستشفى عدن الخيري، موصولًا بجهاز التنفس الصناعي، لا يستطيع أن يبكي بصوت عالٍ مثل باقي الأطفال، لا يصرخ ليطلب الحنان، لا يمد يديه لاحتضان والدته ..
+كل ما يملكه عينان دامعتان، تائهتان، تقولان: أنقذوني.
+💉 هناك أمل.. لكنه بعيد.. بعيد جدًا..
+هناك علاج اسمه "زولجينسما"، حقنة واحدة فقط يمكن أن تُعيد له الحياة، أن تمنحه فرصة ليعيش كغيره من الأطفال .. لكنها تكلف 2.1 مليون دولار.
+🎗️ يا أصحاب السمو أمراء الخليج .. يا رجال المال والأعمال .. يا أهل القلوب الرحيمة.. يا من منحكم الله من فضله..
+كيف يكون المال حاجزًا بين طفل والحياة؟
+كيف يكون ثمن حياة طفل مجرد رقم في الحسابات البنكية؟
+🔹 والده، ثروت عبدالله عنبول، رجل بسيط من حي المنصورة بعدن، يقف بجانب سرير ابنه كل ليلة، يرى قلبه الصغير يقاوم، يرى روحه تتشبث بالحياة، لكنه لا يستطيع فعل شيء سوى الدعاء، وانتظار يد الرحمة التي قد تأتي منكم.
+🔹 لا يوجد وقت..
+⏳ كل يوم يمر، يسرق من مجد فرصة النجاة..
+⏳ كل دقيقة، تضعف عضلاته أكثر..
+⏳ كل لحظة، يقترب أكثر من النهاية.. إلا إذا تحركتم الآن.
+هل ستكون أنت من ينقذ مجد؟
+هل سيكون اسمك مكتوبًا في سجلّ الملائكة كمنقذ لطفل بريء؟
+📞 للتواصل والمساعدة:
+00967733922291 (واتساب)
+🔁 رجاءً، لا تجعلوا هذه المناشدة تتوقف هنا.. انشروها، فربما تصل إلى قلوب رحيمة تنقذه.
+#أنقذوا_مجد
+5h1 likeReply
+See translation
+ah_su.al
+لاسامح التدخلات الخارجية اللي أنهكت البلاد
+6h2 likesReply
+See translation
+yousefsadaqa
+قلوبنا معكم يا اخواننا في اليمن السعيد
+تحية خاصة لكم من ارض الرباط ارض فلسطين💚
+6h49 likesReply
+See translation
+View replies (3)
+hhhhsgga
+@ahmadalshugairi @ahmed_binmubarak @ahmadbinnasser
+5hReply
+6 hours ago
+Post</t>
+        </is>
+      </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>2025-03-12 00:17:24</t>
+          <t>2025-03-12 00:23:48</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -1693,15 +2976,19 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>947b5dd1-016b-47c2-9a7f-bec53fd22042</t>
+          <t>7d704031-9df9-4b9b-b7c2-d552da6cb1ff</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2025-03-11T22:01:44.000Z</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr"/>
+          <t>2025-03-11T15:51:03.000Z</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>459 likes</t>
+        </is>
+      </c>
       <c r="F20" t="inlineStr">
         <is>
           <t>NA</t>
@@ -1712,11 +2999,54 @@
           <t>NA</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>كيف يمكن للقرآن أن يرشد الشباب في اتخاذ قرارات حياتية تفضّل مبادئ الخالق على الضغوط المادية؟
+#الشريعة_والحياة_في_رمضان #الجزيرة_في_رمضان</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>aljazeera
+•
+Follow
+Original audio
+459 likes
+aljazeera
+كيف يمكن للقرآن أن يرشد الشباب في اتخاذ قرارات حياتية تفضّل مبادئ الخالق على الضغوط المادية؟
+#الشريعة_والحياة_في_رمضان #الجزيرة_في_رمضان
+6h
+See translation
+kursatalperen000
+يوم دامٍ في فلسطين.. 10 شهداء في قطاع غزة و5 شهداء بالضفة الغربية واحد منهم برصاص أجهزة أمن السلطة😢
+6h5 likesReply
+See translation
+berghoutim
+مع الاسف في وطننا العربي ،يعترفون بكل الثروات الا الثروة الفكرية
+3h1 likeReply
+See translation
+dr_lena234
+السعاده الزوجيه معنا❤️‍🔥🔥
+6hReply
+See translation
+5zv25
+🖤
+6hReply
+mehdimehdi2310
+شوفوا الاستوري عن امة المليار مع الاسف
+6hReply
+See translation
+joelzedat
+6hReply
+View hidden comments
+These comments were hidden because they may be misleading, offensive or spam. People can still tap to view them.
+6 hours ago
+Post</t>
+        </is>
+      </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>2025-03-12 00:17:39</t>
+          <t>2025-03-12 00:23:53</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -1758,15 +3088,19 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>e8b727b7-56cc-405e-b7d6-b2378e3c46ed</t>
+          <t>283baaf9-31c3-45e8-a5c7-34b9da31c479</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2025-03-11T22:01:44.000Z</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr"/>
+          <t>2025-03-11T15:26:24.000Z</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>1,292 likes</t>
+        </is>
+      </c>
       <c r="F21" t="inlineStr">
         <is>
           <t>NA</t>
@@ -1777,11 +3111,48 @@
           <t>NA</t>
         </is>
       </c>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>قالت وكالة الأنباء الفلسطينية إن مستوطنين أضرموا النيران الثلاثاء، في مستودع سيارات للشقيقين محمد ورأفت السبتي، ما أدى إلى احتراق 3 منها بقرية أم صفا شمال غربي رام الله.
+#فيديو</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>aljazeera
+•
+Follow
+Original audio
+1,292 likes
+aljazeera
+قالت وكالة الأنباء الفلسطينية إن مستوطنين أضرموا النيران الثلاثاء، في مستودع سيارات للشقيقين محمد ورأفت السبتي، ما أدى إلى احتراق 3 منها بقرية أم صفا شمال غربي رام الله.
+#فيديو
+6h
+See translation
+manalhamamy
+يعيثون في الأرض فسادا اللهم ارنا عجائب قدرتك فيهم
+6h5 likesReply
+See translation
+View replies (1)
+salon_ghada
+أنا للة وانا الية راجعون
+6hReply
+joelzedat
+I salute the brave owners of the land for their freedom acts💪♥️🇮🇱
+6hReply
+View replies (19)
+bentoman31
+استقبلي العيد وانتي بيضاء وبشرتكج تجنن 🩷🩷🩷🩷🩷🩷
+6hReply
+See translation
+View replies (1)
+6 hours ago
+Post</t>
+        </is>
+      </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>2025-03-12 00:17:53</t>
+          <t>2025-03-12 00:23:58</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">

</xml_diff>